<commit_message>
Improvements to data generator: * Added mean and stddev to numerical variables to generate normal distributed values * OPAL-1139: generator is aware of continuous variables that also have missing categories * Added ability to generate date values (min and max should be specified as string)
</commit_message>
<xml_diff>
--- a/datasource-generated/src/test/resources/fs.xlsx
+++ b/datasource-generated/src/test/resources/fs.xlsx
@@ -7164,7 +7164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -7191,6 +7191,11 @@
       <family val="2"/>
       <b val="true"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -7240,13 +7245,14 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>

</xml_diff>